<commit_message>
DSA Big O Time Complexity
</commit_message>
<xml_diff>
--- a/Week1/Week1/RunningTime.xlsx
+++ b/Week1/Week1/RunningTime.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nui_t\Google Drive\DataStructure\week0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richard/Desktop/DSA/Week1/Week1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EBC8F4E-BC2B-45E0-8622-9642F709E0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8ECF0C4-7A0D-3D4F-995C-5A9167560F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{CEB7F8C8-D50F-43F1-99EC-D054581DC40D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CEB7F8C8-D50F-43F1-99EC-D054581DC40D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -189,7 +180,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-MM"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -270,6 +261,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.9627999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23682300000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.034807</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8548100000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.953623</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70.535719</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -351,6 +360,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.5322000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.7408999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38969500000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.514867</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.6624349999999897</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.306916999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -432,6 +459,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.8839999999999899E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9579999999999902E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3141999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4188000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9621999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.102267</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -478,6 +523,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.15598100000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.66817700000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.47898</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.108466</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.771323000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>160.245285</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -542,7 +605,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-MM"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="587927280"/>
@@ -601,7 +664,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-MM"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="587923344"/>
@@ -643,7 +706,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-MM"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -680,7 +743,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-MM"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -756,7 +819,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-MM"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -837,6 +900,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.9627999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23682300000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.034807</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8548100000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.953623</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70.535719</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -918,6 +999,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.5322000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.7408999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38969500000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.514867</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.6624349999999897</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.306916999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -999,6 +1098,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.8839999999999899E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9579999999999902E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3141999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4188000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9621999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.102267</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1045,6 +1162,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.15598100000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.66817700000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.47898</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.108466</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.771323000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>160.245285</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1109,7 +1244,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-MM"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="587927280"/>
@@ -1169,7 +1304,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-MM"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="587923344"/>
@@ -1211,7 +1346,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-MM"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1248,7 +1383,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-MM"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2724,15 +2859,15 @@
   <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="7" width="8.7265625" style="1"/>
+    <col min="2" max="7" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2749,52 +2884,124 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1">
         <v>1000</v>
       </c>
+      <c r="D3" s="1">
+        <v>0.15598100000000001</v>
+      </c>
+      <c r="E3" s="1">
+        <v>6.9627999999999995E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2.5322000000000001E-2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2.8839999999999899E-3</v>
+      </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1">
         <v>2000</v>
       </c>
+      <c r="D4" s="1">
+        <v>0.66817700000000002</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.23682300000000001</v>
+      </c>
+      <c r="F4" s="1">
+        <v>9.7408999999999996E-2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5.9579999999999902E-3</v>
+      </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1">
         <v>4000</v>
       </c>
+      <c r="D5" s="1">
+        <v>2.47898</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.034807</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.38969500000000001</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1.3141999999999999E-2</v>
+      </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1">
         <v>8000</v>
       </c>
+      <c r="D6" s="1">
+        <v>11.108466</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3.8548100000000001</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.514867</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2.4188000000000001E-2</v>
+      </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1">
         <v>16000</v>
       </c>
+      <c r="D7" s="1">
+        <v>40.771323000000002</v>
+      </c>
+      <c r="E7" s="1">
+        <v>16.953623</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6.6624349999999897</v>
+      </c>
+      <c r="G7" s="1">
+        <v>4.9621999999999999E-2</v>
+      </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>32000</v>
+      </c>
+      <c r="D8" s="1">
+        <v>160.245285</v>
+      </c>
+      <c r="E8" s="1">
+        <v>70.535719</v>
+      </c>
+      <c r="F8" s="1">
+        <v>24.306916999999999</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.102267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>